<commit_message>
so much joy today
Signed-off-by: ibicdlcod <504161487@qq.com>
</commit_message>
<xml_diff>
--- a/doc/Tech level.xlsx
+++ b/doc/Tech level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GuoMuoRuoProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6E3306-24D6-41CA-9F25-B145EB570293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2AC706-181A-4BFE-BA28-09ABF197AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -774,7 +774,7 @@
     <col min="7" max="7" width="50.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.06640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.06640625" style="1"/>
   </cols>
@@ -825,11 +825,11 @@
       </c>
       <c r="J2" s="1">
         <f ca="1">RAND()*10</f>
-        <v>1.2797161622568698</v>
+        <v>8.1413445901349366</v>
       </c>
       <c r="K2" s="1">
         <f ca="1">I2*($H$1^J2-1)*$H$1^(-SUM($J$2:J2))</f>
-        <v>0.12511667793487574</v>
+        <v>0.74447601639822114</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -856,11 +856,11 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" ca="1" si="1">RAND()*10</f>
-        <v>6.167111679742967</v>
+        <v>9.6783987049559546</v>
       </c>
       <c r="K3" s="1">
         <f ca="1">I3*($H$1^J3-1)*$H$1^(-SUM($J$2:J3))</f>
-        <v>0.54921915026093393</v>
+        <v>0.72736431765883525</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -887,11 +887,11 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6399114948877278</v>
+        <v>5.8554915251180342</v>
       </c>
       <c r="K4" s="1">
         <f ca="1">I4*($H$1^J4-1)*$H$1^(-SUM($J$2:J4))</f>
-        <v>0.2109633561514079</v>
+        <v>0.3692654820921582</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -918,11 +918,11 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3710531789574993</v>
+        <v>5.7316422115751609</v>
       </c>
       <c r="K5" s="1">
         <f ca="1">I5*($H$1^J5-1)*$H$1^(-SUM($J$2:J5))</f>
-        <v>0.17654622506580059</v>
+        <v>0.31555509585784036</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -949,11 +949,11 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9.302690891959088</v>
+        <v>0.91856485941427701</v>
       </c>
       <c r="K6" s="1">
         <f ca="1">I6*($H$1^J6-1)*$H$1^(-SUM($J$2:J6))</f>
-        <v>0.60473016518872302</v>
+        <v>4.6317206543944139E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -980,11 +980,11 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3062811401834917</v>
+        <v>6.063258879861662</v>
       </c>
       <c r="K7" s="1">
         <f ca="1">I7*($H$1^J7-1)*$H$1^(-SUM($J$2:J7))</f>
-        <v>0.4435778134222752</v>
+        <v>0.27927093484001808</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -1011,11 +1011,11 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0201252971145669</v>
+        <v>1.5715917856549233</v>
       </c>
       <c r="K8" s="1">
         <f ca="1">I8*($H$1^J8-1)*$H$1^(-SUM($J$2:J8))</f>
-        <v>4.8514373375657331E-2</v>
+        <v>6.5588199713233611E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -1042,11 +1042,11 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.157481309473245</v>
+        <v>3.0752708608545043</v>
       </c>
       <c r="K9" s="1">
         <f ca="1">I9*($H$1^J9-1)*$H$1^(-SUM($J$2:J9))</f>
-        <v>0.22557318101580617</v>
+        <v>0.11979888754509506</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
@@ -1073,11 +1073,11 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8567712976222737</v>
+        <v>0.83885018915789478</v>
       </c>
       <c r="K10" s="1">
         <f ca="1">I10*($H$1^J10-1)*$H$1^(-SUM($J$2:J10))</f>
-        <v>0.1506639232953545</v>
+        <v>3.070021964225797E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="J11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4538155283880223</v>
+        <v>5.0310203416177259</v>
       </c>
       <c r="K11" s="1">
         <f ca="1">I11*($H$1^J11-1)*$H$1^(-SUM($J$2:J11))</f>
-        <v>0.12250731926582407</v>
+        <v>0.1696607451245867</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -1132,11 +1132,11 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8827024486641246</v>
+        <v>6.3835320154163044</v>
       </c>
       <c r="K12" s="1">
         <f ca="1">I12*($H$1^J12-1)*$H$1^(-SUM($J$2:J12))</f>
-        <v>0.15560948583176992</v>
+        <v>0.1876240233912749</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
@@ -1160,11 +1160,11 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6.251456408812829</v>
+        <v>8.0037871315823779</v>
       </c>
       <c r="K13" s="1">
         <f ca="1">I13*($H$1^J13-1)*$H$1^(-SUM($J$2:J13))</f>
-        <v>0.17401709469833679</v>
+        <v>0.19898768628832242</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9.314539798334863</v>
+        <v>5.870147419799042</v>
       </c>
       <c r="K14" s="1">
         <f ca="1">I14*($H$1^J14-1)*$H$1^(-SUM($J$2:J14))</f>
-        <v>0.21671759870970467</v>
+        <v>0.12388809351186357</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1216,11 +1216,11 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3171674837434166</v>
+        <v>7.6282852693464518</v>
       </c>
       <c r="K15" s="1">
         <f ca="1">I15*($H$1^J15-1)*$H$1^(-SUM($J$2:J15))</f>
-        <v>2.6820784465432901E-2</v>
+        <v>0.13719855869591707</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44130181065619167</v>
+        <v>1.3775706633874207</v>
       </c>
       <c r="K16" s="1">
         <f ca="1">I16*($H$1^J16-1)*$H$1^(-SUM($J$2:J16))</f>
-        <v>8.5920038516024873E-3</v>
+        <v>2.2029870792783329E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
@@ -1272,11 +1272,11 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0817734681847311</v>
+        <v>6.9758106293860251</v>
       </c>
       <c r="K17" s="1">
         <f ca="1">I17*($H$1^J17-1)*$H$1^(-SUM($J$2:J17))</f>
-        <v>0.12452911365450332</v>
+        <v>9.9924002499447953E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
@@ -1300,11 +1300,11 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5264831770690768</v>
+        <v>9.4660543260481589</v>
       </c>
       <c r="K18" s="1">
         <f ca="1">I18*($H$1^J18-1)*$H$1^(-SUM($J$2:J18))</f>
-        <v>2.3926337946440546E-2</v>
+        <v>0.11200669579292191</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
@@ -1328,11 +1328,11 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3000450610494563</v>
+        <v>9.4720681489716956</v>
       </c>
       <c r="K19" s="1">
         <f ca="1">I19*($H$1^J19-1)*$H$1^(-SUM($J$2:J19))</f>
-        <v>1.923174902905098E-2</v>
+        <v>9.018204610497374E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
@@ -1356,11 +1356,11 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6424552125903631</v>
+        <v>7.9775494587053677</v>
       </c>
       <c r="K20" s="1">
         <f ca="1">I20*($H$1^J20-1)*$H$1^(-SUM($J$2:J20))</f>
-        <v>7.5600573880906657E-2</v>
+        <v>6.1938544499715774E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
@@ -1384,11 +1384,11 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2874989258074221</v>
+        <v>6.1018145277680951</v>
       </c>
       <c r="K21" s="1">
         <f ca="1">I21*($H$1^J21-1)*$H$1^(-SUM($J$2:J21))</f>
-        <v>7.252727790028915E-2</v>
+        <v>3.9905466691906533E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
@@ -1412,11 +1412,11 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4401413192050427</v>
+        <v>5.453565355687223</v>
       </c>
       <c r="K22" s="1">
         <f ca="1">I22*($H$1^J22-1)*$H$1^(-SUM($J$2:J22))</f>
-        <v>1.4883080664274255E-2</v>
+        <v>3.0780183547053606E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
@@ -1440,11 +1440,11 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3520342760901567</v>
+        <v>5.9576511212799499</v>
       </c>
       <c r="K23" s="1">
         <f ca="1">I23*($H$1^J23-1)*$H$1^(-SUM($J$2:J23))</f>
-        <v>5.001093123305185E-2</v>
+        <v>2.903448268789029E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
@@ -1468,11 +1468,11 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5271718463899653</v>
+        <v>4.5290168588167887</v>
       </c>
       <c r="K24" s="1">
         <f ca="1">I24*($H$1^J24-1)*$H$1^(-SUM($J$2:J24))</f>
-        <v>6.7102999760008192E-2</v>
+        <v>1.9204505618908244E-2</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
@@ -1496,11 +1496,11 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5894814739538945</v>
+        <v>5.2246753398517409</v>
       </c>
       <c r="K25" s="1">
         <f ca="1">I25*($H$1^J25-1)*$H$1^(-SUM($J$2:J25))</f>
-        <v>4.082225906928293E-3</v>
+        <v>1.9398612275038814E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
@@ -1524,11 +1524,11 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6844763146058286</v>
+        <v>7.9568207825723078</v>
       </c>
       <c r="K26" s="1">
         <f ca="1">I26*($H$1^J26-1)*$H$1^(-SUM($J$2:J26))</f>
-        <v>3.5643075388499132E-2</v>
+        <v>2.4982415654542064E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
@@ -1548,11 +1548,11 @@
       </c>
       <c r="J27" s="1">
         <f ca="1">SUM(J2:J26)</f>
-        <v>109.19368700574313</v>
+        <v>145.28378299696402</v>
       </c>
       <c r="K27" s="1">
         <f ca="1">SUM(K2:K26)</f>
-        <v>3.7267065178974574</v>
+        <v>4.0650822934687509</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="K40" s="1">
         <f ca="1">SUM(K2:K39)</f>
-        <v>7.4534130357949149</v>
+        <v>8.1301645869375019</v>
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
cal tech is functional
Signed-off-by: ibicdlcod <504161487@qq.com>
</commit_message>
<xml_diff>
--- a/doc/Tech level.xlsx
+++ b/doc/Tech level.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GuoMuoRuoProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28434FAF-4175-44CC-A0DA-3F374769601A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C271BB3-5838-4B9E-9E55-F3F85A210C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="11993" yWindow="0" windowWidth="7499" windowHeight="6000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
   <si>
     <t>1st</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -826,11 +826,11 @@
       </c>
       <c r="J2" s="1">
         <f ca="1">RAND()*10</f>
-        <v>5.5077196943109028</v>
+        <v>8.3520069650172033</v>
       </c>
       <c r="K2" s="1">
         <f ca="1">I2*($H$1^J2-1)*$H$1^(-SUM($J$2:J2))</f>
-        <v>0.51664974341390413</v>
+        <v>0.76219167411340982</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -857,11 +857,11 @@
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" ca="1" si="1">RAND()*10</f>
-        <v>7.5131114787449498</v>
+        <v>6.8906818317937262</v>
       </c>
       <c r="K3" s="1">
         <f ca="1">I3*($H$1^J3-1)*$H$1^(-SUM($J$2:J3))</f>
-        <v>0.60738609360335816</v>
+        <v>0.52973510412588709</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -888,11 +888,11 @@
       </c>
       <c r="J4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1760333967601628</v>
+        <v>6.6148673132520592</v>
       </c>
       <c r="K4" s="1">
         <f ca="1">I4*($H$1^J4-1)*$H$1^(-SUM($J$2:J4))</f>
-        <v>0.36133700875056318</v>
+        <v>0.4357740894574238</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -919,11 +919,11 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2990397681700969</v>
+        <v>4.5409692650128273</v>
       </c>
       <c r="K5" s="1">
         <f ca="1">I5*($H$1^J5-1)*$H$1^(-SUM($J$2:J5))</f>
-        <v>0.38440937459915753</v>
+        <v>0.26218645628322873</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -950,11 +950,11 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6672206115138382</v>
+        <v>3.7696579594463628</v>
       </c>
       <c r="K6" s="1">
         <f ca="1">I6*($H$1^J6-1)*$H$1^(-SUM($J$2:J6))</f>
-        <v>0.25000868944165161</v>
+        <v>0.19617412269934326</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -981,11 +981,11 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3499054860020898</v>
+        <v>7.7572592718847053</v>
       </c>
       <c r="K7" s="1">
         <f ca="1">I7*($H$1^J7-1)*$H$1^(-SUM($J$2:J7))</f>
-        <v>0.2539051921230287</v>
+        <v>0.35258360876676836</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -1012,11 +1012,11 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7799106284259967</v>
+        <v>3.9728173365282671</v>
       </c>
       <c r="K8" s="1">
         <f ca="1">I8*($H$1^J8-1)*$H$1^(-SUM($J$2:J8))</f>
-        <v>0.11898420588834979</v>
+        <v>0.15708593630341339</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3185969999911116</v>
+        <v>9.9365487463797368</v>
       </c>
       <c r="K9" s="1">
         <f ca="1">I9*($H$1^J9-1)*$H$1^(-SUM($J$2:J9))</f>
-        <v>0.31205842018420743</v>
+        <v>0.33501711747048912</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
@@ -1074,11 +1074,11 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35347914128540769</v>
+        <v>4.8668134207962357</v>
       </c>
       <c r="K10" s="1">
         <f ca="1">I10*($H$1^J10-1)*$H$1^(-SUM($J$2:J10))</f>
-        <v>1.1872706439020499E-2</v>
+        <v>0.13825119420028048</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -1102,11 +1102,11 @@
       </c>
       <c r="J11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0205397610239948</v>
+        <v>8.4051560009835455</v>
       </c>
       <c r="K11" s="1">
         <f ca="1">I11*($H$1^J11-1)*$H$1^(-SUM($J$2:J11))</f>
-        <v>9.5798860729749954E-2</v>
+        <v>0.20453473182685664</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -1133,11 +1133,11 @@
       </c>
       <c r="J12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0555938219642147</v>
+        <v>6.938308459330278</v>
       </c>
       <c r="K12" s="1">
         <f ca="1">I12*($H$1^J12-1)*$H$1^(-SUM($J$2:J12))</f>
-        <v>3.1366365871419985E-2</v>
+        <v>0.14145332627189111</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
@@ -1161,11 +1161,11 @@
       </c>
       <c r="J13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4980569314327887</v>
+        <v>6.5269519205159954</v>
       </c>
       <c r="K13" s="1">
         <f ca="1">I13*($H$1^J13-1)*$H$1^(-SUM($J$2:J13))</f>
-        <v>0.24823168064063023</v>
+        <v>0.11353598191251682</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
@@ -1189,11 +1189,11 @@
       </c>
       <c r="J14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65338686257762846</v>
+        <v>2.8496333467639778</v>
       </c>
       <c r="K14" s="1">
         <f ca="1">I14*($H$1^J14-1)*$H$1^(-SUM($J$2:J14))</f>
-        <v>1.5025288000698449E-2</v>
+        <v>4.3991251913430091E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1217,11 +1217,11 @@
       </c>
       <c r="J15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59391431170679909</v>
+        <v>4.1615986238746991</v>
       </c>
       <c r="K15" s="1">
         <f ca="1">I15*($H$1^J15-1)*$H$1^(-SUM($J$2:J15))</f>
-        <v>1.3135006643415719E-2</v>
+        <v>5.8367625262740176E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -1245,11 +1245,11 @@
       </c>
       <c r="J16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83068015714958032</v>
+        <v>7.0508843681969156</v>
       </c>
       <c r="K16" s="1">
         <f ca="1">I16*($H$1^J16-1)*$H$1^(-SUM($J$2:J16))</f>
-        <v>1.7624533641995978E-2</v>
+        <v>8.6153196796766404E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
@@ -1273,11 +1273,11 @@
       </c>
       <c r="J17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6525569895384411</v>
+        <v>3.874688385068159</v>
       </c>
       <c r="K17" s="1">
         <f ca="1">I17*($H$1^J17-1)*$H$1^(-SUM($J$2:J17))</f>
-        <v>7.208714185477029E-2</v>
+        <v>4.1286021400445863E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
@@ -1301,11 +1301,11 @@
       </c>
       <c r="J18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7247052701077399</v>
+        <v>3.4220660814564141</v>
       </c>
       <c r="K18" s="1">
         <f ca="1">I18*($H$1^J18-1)*$H$1^(-SUM($J$2:J18))</f>
-        <v>4.9037288637617221E-2</v>
+        <v>3.295075818303652E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
@@ -1329,11 +1329,11 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5659700494069559</v>
+        <v>2.8738979263327327</v>
       </c>
       <c r="K19" s="1">
         <f ca="1">I19*($H$1^J19-1)*$H$1^(-SUM($J$2:J19))</f>
-        <v>5.8533802555100899E-2</v>
+        <v>2.5233977266955112E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
@@ -1357,11 +1357,11 @@
       </c>
       <c r="J20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.266676011593288</v>
+        <v>6.2013558655370264</v>
       </c>
       <c r="K20" s="1">
         <f ca="1">I20*($H$1^J20-1)*$H$1^(-SUM($J$2:J20))</f>
-        <v>4.8593219503142604E-2</v>
+        <v>4.8286635046153936E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
@@ -1385,11 +1385,11 @@
       </c>
       <c r="J21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.6467330702151171</v>
+        <v>6.6108491901289925</v>
       </c>
       <c r="K21" s="1">
         <f ca="1">I21*($H$1^J21-1)*$H$1^(-SUM($J$2:J21))</f>
-        <v>3.5969739313164911E-2</v>
+        <v>4.3929159173986626E-2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3570092893212271</v>
+        <v>0.2223746912855451</v>
       </c>
       <c r="K22" s="1">
         <f ca="1">I22*($H$1^J22-1)*$H$1^(-SUM($J$2:J22))</f>
-        <v>6.5109781833582792E-2</v>
+        <v>1.3355107343165399E-3</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
@@ -1441,11 +1441,11 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55134773371599999</v>
+        <v>4.1708355445113989</v>
       </c>
       <c r="K23" s="1">
         <f ca="1">I23*($H$1^J23-1)*$H$1^(-SUM($J$2:J23))</f>
-        <v>6.106864318570022E-3</v>
+        <v>2.3189625623197388E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4401667851922682</v>
+        <v>0.63693946083075992</v>
       </c>
       <c r="K24" s="1">
         <f ca="1">I24*($H$1^J24-1)*$H$1^(-SUM($J$2:J24))</f>
-        <v>2.533661240880327E-2</v>
+        <v>3.2593759644541222E-3</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
@@ -1497,11 +1497,11 @@
       </c>
       <c r="J25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5849954540415556</v>
+        <v>7.5166141297337177</v>
       </c>
       <c r="K25" s="1">
         <f ca="1">I25*($H$1^J25-1)*$H$1^(-SUM($J$2:J25))</f>
-        <v>4.2832338932068621E-2</v>
+        <v>3.4245324285932056E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
@@ -1525,11 +1525,11 @@
       </c>
       <c r="J26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4578779271469422</v>
+        <v>2.3577950474961904</v>
       </c>
       <c r="K26" s="1">
         <f ca="1">I26*($H$1^J26-1)*$H$1^(-SUM($J$2:J26))</f>
-        <v>2.0616337570908125E-2</v>
+        <v>9.3728669312552366E-3</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
@@ -1549,11 +1549,11 @@
       </c>
       <c r="J27" s="1">
         <f ca="1">SUM(J2:J26)</f>
-        <v>92.865227631339096</v>
+        <v>130.52157115215743</v>
       </c>
       <c r="K27" s="1">
         <f ca="1">SUM(K2:K26)</f>
-        <v>3.6620162968988805</v>
+        <v>4.0801246720141782</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="K40" s="1">
         <f ca="1">SUM(K2:K39)</f>
-        <v>7.3240325937977611</v>
+        <v>8.1602493440283563</v>
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.4">
@@ -2273,4 +2273,281 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F99C48-C805-4C9F-AD1F-EA5EFE25C650}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2*($A$1^C2-1)*$A$1^(-SUM(C$2:$C2))</f>
+        <v>0.17303299635886632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>B3*($A$1^C3-1)*$A$1^(-SUM(C$2:$C3))</f>
+        <v>7.3183049434257186E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <f>B4*($A$1^C4-1)*$A$1^(-SUM(C$2:$C4))</f>
+        <v>1.7759427643723857E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <f>B5*($A$1^C5-1)*$A$1^(-SUM(C$2:$C5))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <f>B6*($A$1^C6-1)*$A$1^(-SUM(C$2:$C6))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <f>B7*($A$1^C7-1)*$A$1^(-SUM(C$2:$C7))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <f>B8*($A$1^C8-1)*$A$1^(-SUM(C$2:$C8))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <f>B9*($A$1^C9-1)*$A$1^(-SUM(C$2:$C9))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <f>B10*($A$1^C10-1)*$A$1^(-SUM(C$2:$C10))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f>B11*($A$1^C11-1)*$A$1^(-SUM(C$2:$C11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <f>B12*($A$1^C12-1)*$A$1^(-SUM(C$2:$C12))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <f>B13*($A$1^C13-1)*$A$1^(-SUM(C$2:$C13))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <f>B14*($A$1^C14-1)*$A$1^(-SUM(C$2:$C14))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <f>B15*($A$1^C15-1)*$A$1^(-SUM(C$2:$C15))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1">
+        <f>B16*($A$1^C16-1)*$A$1^(-SUM(C$2:$C16))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <f>B17*($A$1^C17-1)*$A$1^(-SUM(C$2:$C17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <f>B18*($A$1^C18-1)*$A$1^(-SUM(C$2:$C18))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <f>B19*($A$1^C19-1)*$A$1^(-SUM(C$2:$C19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <f>B20*($A$1^C20-1)*$A$1^(-SUM(C$2:$C20))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <f>B21*($A$1^C21-1)*$A$1^(-SUM(C$2:$C21))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <f>B22*($A$1^C22-1)*$A$1^(-SUM(C$2:$C22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <f>B23*($A$1^C23-1)*$A$1^(-SUM(C$2:$C23))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <f>B24*($A$1^C24-1)*$A$1^(-SUM(C$2:$C24))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <f>B25*($A$1^C25-1)*$A$1^(-SUM(C$2:$C25))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <f>B26*($A$1^C26-1)*$A$1^(-SUM(C$2:$C26))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1">
+        <f>SUM(C2:C26)</f>
+        <v>6</v>
+      </c>
+      <c r="D27" s="1">
+        <f>SUM(D2:D26)</f>
+        <v>0.26397547343684735</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>